<commit_message>
Fix RGBLED partnumber on Mini-HUB BOM
</commit_message>
<xml_diff>
--- a/Mini HUB/PCB/Chordata Mini HUB BOM v1.3.xlsx
+++ b/Mini HUB/PCB/Chordata Mini HUB BOM v1.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\chordata\Mini HUB\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E3EA4F-ECA7-4C55-95A5-F68BFCC8E4C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA56C46-EC25-4103-BBBC-2523056D413F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="375" yWindow="17145" windowWidth="29835" windowHeight="14565" xr2:uid="{876730CE-73A8-4045-9E1B-47206136867B}"/>
   </bookViews>
@@ -220,10 +220,10 @@
     <t>Quantity in a set</t>
   </si>
   <si>
-    <t>584-LTC4316CMS#PBF (sold in strip of 10)</t>
-  </si>
-  <si>
     <t>C114586 (minimum 5)</t>
+  </si>
+  <si>
+    <t>COM-13667 (sold in strip of 10)</t>
   </si>
 </sst>
 </file>
@@ -601,6 +601,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -644,39 +677,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -998,8 +998,8 @@
   </sheetPr>
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,88 +1011,88 @@
     <col min="5" max="5" width="42.140625" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="14" max="14" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="36" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="47" t="s">
         <v>4</v>
       </c>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="39" t="s">
+      <c r="A3" s="46"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="39" t="s">
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="39" t="s">
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="40"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="37"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="48"/>
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="46"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="42" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="19" t="s">
@@ -1113,7 +1113,7 @@
       <c r="M4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="37"/>
+      <c r="N4" s="48"/>
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1166,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F6" s="5">
         <v>4.95</v>
@@ -1179,7 +1179,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="18"/>
       <c r="K6" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L6">
         <v>0.1</v>
@@ -1192,36 +1192,36 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="47">
+    <row r="7" spans="1:15" s="38" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
         <v>3</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="35">
         <v>6</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="37">
         <v>1.03</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="38">
         <f>IF(F7&gt;0,F7*$D7,"")</f>
         <v>6.18</v>
       </c>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="55" t="s">
+      <c r="H7" s="36"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="40" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1452,36 +1452,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="53" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="47">
+    <row r="15" spans="1:15" s="38" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="32">
         <v>11</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="35">
         <v>17</v>
       </c>
-      <c r="E15" s="51" t="s">
+      <c r="E15" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="52">
+      <c r="F15" s="37">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="G15" s="54">
+      <c r="G15" s="39">
         <f t="shared" si="2"/>
         <v>1.0029999999999999</v>
       </c>
-      <c r="H15" s="51"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="52"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="37"/>
       <c r="M15" s="18"/>
-      <c r="N15" s="55" t="s">
+      <c r="N15" s="40" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1502,7 +1502,7 @@
       <c r="K16" s="17"/>
       <c r="L16" s="5"/>
       <c r="M16" s="18" t="str">
-        <f t="shared" ref="M9:M16" si="3">IF(L16&gt;0,L16*$D16,"")</f>
+        <f t="shared" ref="M16" si="3">IF(L16&gt;0,L16*$D16,"")</f>
         <v/>
       </c>
       <c r="N16" s="6"/>

</xml_diff>

<commit_message>
Fixed LED pipe part number;
</commit_message>
<xml_diff>
--- a/Mini HUB/PCB/Chordata Mini HUB BOM v1.3.xlsx
+++ b/Mini HUB/PCB/Chordata Mini HUB BOM v1.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\chordata\Mini HUB\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA56C46-EC25-4103-BBBC-2523056D413F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631BE6E0-5DC6-46FC-B69C-E4533A062C9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="17145" windowWidth="29835" windowHeight="14565" xr2:uid="{876730CE-73A8-4045-9E1B-47206136867B}"/>
+    <workbookView xWindow="7755" yWindow="7755" windowWidth="23985" windowHeight="21495" xr2:uid="{876730CE-73A8-4045-9E1B-47206136867B}"/>
   </bookViews>
   <sheets>
     <sheet name="Mini HUB v1.3" sheetId="1" r:id="rId1"/>
@@ -135,13 +135,7 @@
     <t>SMD</t>
   </si>
   <si>
-    <t>VLP-200-R</t>
-  </si>
-  <si>
     <t>LEDPIPE</t>
-  </si>
-  <si>
-    <t>749-VLP-200-R</t>
   </si>
   <si>
     <t>-</t>
@@ -224,6 +218,12 @@
   </si>
   <si>
     <t>COM-13667 (sold in strip of 10)</t>
+  </si>
+  <si>
+    <t>VLP-500-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">749-VLP-500-R </t>
   </si>
 </sst>
 </file>
@@ -999,7 +999,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1020,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -1040,7 +1040,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="56" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="53" t="s">
         <v>1</v>
@@ -1096,7 +1096,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I4" s="20" t="s">
         <v>8</v>
@@ -1121,16 +1121,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>49</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>51</v>
       </c>
       <c r="D5" s="24">
         <v>1</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" s="26">
         <v>1.0900000000000001</v>
@@ -1149,7 +1149,7 @@
         <v/>
       </c>
       <c r="N5" s="28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1157,16 +1157,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="D6" s="11">
         <v>1</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" s="5">
         <v>4.95</v>
@@ -1179,7 +1179,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="18"/>
       <c r="K6" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L6">
         <v>0.1</v>
@@ -1200,7 +1200,7 @@
         <v>31</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="35">
         <v>6</v>
@@ -1230,23 +1230,23 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D8" s="11">
         <v>3</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>36</v>
+      <c r="E8" t="s">
+        <v>56</v>
       </c>
       <c r="F8" s="5">
-        <v>0.158</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G8">
         <f t="shared" ref="G8" si="1">IF(F8&gt;0,F8*$D8,"")</f>
-        <v>0.47399999999999998</v>
+        <v>1.6500000000000001</v>
       </c>
       <c r="H8" s="17"/>
       <c r="I8" s="5"/>
@@ -1255,7 +1255,7 @@
       <c r="L8" s="5"/>
       <c r="M8" s="18"/>
       <c r="N8" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1263,10 +1263,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9" s="11">
         <v>1</v>
@@ -1427,7 +1427,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="11">
         <v>2</v>
@@ -1460,7 +1460,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="35">
         <v>17</v>
@@ -1514,15 +1514,15 @@
       <c r="D17" s="11"/>
       <c r="E17" s="17"/>
       <c r="F17" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G17" s="18">
         <f>SUM(G5:G15)</f>
-        <v>18.581</v>
+        <v>19.756999999999998</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J17" s="18">
         <f>SUM(J5:J15)</f>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="K17" s="17"/>
       <c r="L17" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M17" s="18">
         <f>SUM(M5:M15)</f>

</xml_diff>

<commit_message>
Removed unused capacitor from the Mini-Hub BOM
</commit_message>
<xml_diff>
--- a/Mini HUB/PCB/Chordata Mini HUB BOM v1.3.xlsx
+++ b/Mini HUB/PCB/Chordata Mini HUB BOM v1.3.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\chordata\Mini HUB\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631BE6E0-5DC6-46FC-B69C-E4533A062C9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6252A48-1088-4BCD-AFDA-7D159EF367A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7755" yWindow="7755" windowWidth="23985" windowHeight="21495" xr2:uid="{876730CE-73A8-4045-9E1B-47206136867B}"/>
+    <workbookView xWindow="13245" yWindow="2655" windowWidth="40800" windowHeight="28410" xr2:uid="{876730CE-73A8-4045-9E1B-47206136867B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mini HUB v1.3" sheetId="1" r:id="rId1"/>
+    <sheet name="Mini HUB v1.3.1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Item</t>
   </si>
@@ -99,21 +93,9 @@
     <t>SMD, 0805</t>
   </si>
   <si>
-    <t>710-885012207098</t>
-  </si>
-  <si>
-    <t>Generic 0805 MLCC 100nF</t>
-  </si>
-  <si>
-    <t>Generic 0805 MLCC 10nF</t>
-  </si>
-  <si>
     <t>Generic 1206 MLCC 10uF</t>
   </si>
   <si>
-    <t>710-885012207092</t>
-  </si>
-  <si>
     <t>SMD, 1206</t>
   </si>
   <si>
@@ -151,6 +133,57 @@
   </si>
   <si>
     <t>LCSC total</t>
+  </si>
+  <si>
+    <t>CN1,CN2,CN3,CN4,CN5,CN6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">649-1012938390601ALF </t>
+  </si>
+  <si>
+    <t>R5,R6,R1,R2,R3,R4,R7,R8,R9,R10,R11,R12,R13,R14,R15,R16,R17</t>
+  </si>
+  <si>
+    <t>WS2812B</t>
+  </si>
+  <si>
+    <t>HEADER-SBC</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>PCA9548ABS,118</t>
+  </si>
+  <si>
+    <t>771-PCA9548ABS118</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>C7,C6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD, HVQFN-24 </t>
+  </si>
+  <si>
+    <t>Quantity in a set</t>
+  </si>
+  <si>
+    <t>C114586 (minimum 5)</t>
+  </si>
+  <si>
+    <t>COM-13667 (sold in strip of 10)</t>
+  </si>
+  <si>
+    <t>VLP-500-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">749-VLP-500-R </t>
+  </si>
+  <si>
+    <t>&lt;removed&gt;</t>
   </si>
   <si>
     <r>
@@ -162,7 +195,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Chordata Mini HUB Bill of Materials - v1.3
+      <t xml:space="preserve">Chordata Mini HUB Bill of Materials - v1.3.1
 </t>
     </r>
     <r>
@@ -177,54 +210,6 @@
       <t>2020 Valor</t>
     </r>
   </si>
-  <si>
-    <t>CN1,CN2,CN3,CN4,CN5,CN6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">649-1012938390601ALF </t>
-  </si>
-  <si>
-    <t>R5,R6,R1,R2,R3,R4,R7,R8,R9,R10,R11,R12,R13,R14,R15,R16,R17</t>
-  </si>
-  <si>
-    <t>WS2812B</t>
-  </si>
-  <si>
-    <t>HEADER-SBC</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>PCA9548ABS,118</t>
-  </si>
-  <si>
-    <t>771-PCA9548ABS118</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>C7,C6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD, HVQFN-24 </t>
-  </si>
-  <si>
-    <t>Quantity in a set</t>
-  </si>
-  <si>
-    <t>C114586 (minimum 5)</t>
-  </si>
-  <si>
-    <t>COM-13667 (sold in strip of 10)</t>
-  </si>
-  <si>
-    <t>VLP-500-R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">749-VLP-500-R </t>
-  </si>
 </sst>
 </file>
 
@@ -233,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +255,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -544,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -678,6 +671,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -999,7 +995,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1016,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -1040,7 +1036,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="56" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E2" s="53" t="s">
         <v>1</v>
@@ -1096,7 +1092,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I4" s="20" t="s">
         <v>8</v>
@@ -1121,16 +1117,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D5" s="24">
         <v>1</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F5" s="26">
         <v>1.0900000000000001</v>
@@ -1149,7 +1145,7 @@
         <v/>
       </c>
       <c r="N5" s="28" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1157,16 +1153,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D6" s="11">
         <v>1</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F6" s="5">
         <v>4.95</v>
@@ -1179,7 +1175,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="18"/>
       <c r="K6" s="17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="L6">
         <v>0.1</v>
@@ -1189,7 +1185,7 @@
         <v>0.1</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="38" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1197,16 +1193,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D7" s="35">
         <v>6</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F7" s="37">
         <v>1.03</v>
@@ -1222,7 +1218,7 @@
       <c r="L7" s="37"/>
       <c r="M7" s="39"/>
       <c r="N7" s="40" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1230,16 +1226,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="11">
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F8" s="5">
         <v>0.55000000000000004</v>
@@ -1255,7 +1251,7 @@
       <c r="L8" s="5"/>
       <c r="M8" s="18"/>
       <c r="N8" s="16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1263,10 +1259,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D9" s="11">
         <v>1</v>
@@ -1361,79 +1357,57 @@
       <c r="A12" s="13">
         <v>8</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>23</v>
+      <c r="B12" s="58" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="11">
-        <v>45</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="5">
-        <v>6.2E-2</v>
-      </c>
-      <c r="G12" s="18">
-        <f t="shared" si="2"/>
-        <v>2.79</v>
-      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="17"/>
       <c r="I12" s="5"/>
       <c r="J12" s="18"/>
       <c r="K12" s="17"/>
       <c r="L12" s="5"/>
       <c r="M12" s="18"/>
-      <c r="N12" s="16" t="s">
-        <v>21</v>
-      </c>
+      <c r="N12" s="16"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>9</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
+      <c r="B13" s="58" t="s">
+        <v>52</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="11">
-        <v>15</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="G13" s="18">
-        <f t="shared" si="2"/>
-        <v>1.2</v>
-      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="17"/>
       <c r="I13" s="5"/>
       <c r="J13" s="18"/>
       <c r="K13" s="17"/>
       <c r="L13" s="5"/>
       <c r="M13" s="18"/>
-      <c r="N13" s="16" t="s">
-        <v>21</v>
-      </c>
+      <c r="N13" s="16"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D14" s="11">
         <v>2</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F14" s="5">
         <v>0.13800000000000001</v>
@@ -1449,7 +1423,7 @@
       <c r="L14" s="5"/>
       <c r="M14" s="18"/>
       <c r="N14" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="38" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1457,16 +1431,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D15" s="35">
         <v>17</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F15" s="37">
         <v>5.8999999999999997E-2</v>
@@ -1514,15 +1488,15 @@
       <c r="D17" s="11"/>
       <c r="E17" s="17"/>
       <c r="F17" s="15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G17" s="18">
         <f>SUM(G5:G15)</f>
-        <v>19.756999999999998</v>
+        <v>15.766999999999999</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J17" s="18">
         <f>SUM(J5:J15)</f>
@@ -1530,7 +1504,7 @@
       </c>
       <c r="K17" s="17"/>
       <c r="L17" s="15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M17" s="18">
         <f>SUM(M5:M15)</f>

</xml_diff>